<commit_message>
Update 4. Codext - Matriz de transición.xlsx
Correcciones de en la columna Token:
Se cambio de PR16 a PR05
Se cambio de PE19 a PR19

Correcciones en el estado:
+ estado 0: 122 -> 130
_ estado 0: 124 -> 132
/ estado 0: 128 -> 136
% estado 0: 130 -> 138
= estado 0: 132 -> 140
& estado 0: 134 -> 142
| estado 0: 136 -> 144
! estado 0: 138 -> 146
> estado 0: 140 -> 148
(*) estado 0: 144 -> 152
# estado 0: 148 -> 156
. estado 0: 150 -> 158
, estado 0: 152 -> 160
" estado 0: 154 -> 162
( estado 0: 156 -> 164
) estado 0: 158 -> 166
Δ estado 0: 160 -> 168
\n estado 0: 162 -> 170

POSIBLE CORRECCIÓN: En la columna AV de excel esta la columna A/n, revisar si cambiar a A\n no afectaría al programa.
</commit_message>
<xml_diff>
--- a/docs/Documentación/4. Codext - Matriz de transición.xlsx
+++ b/docs/Documentación/4. Codext - Matriz de transición.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asduf\Documents\GitHub\Codext\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Codext\docs\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97496E95-99A7-43E0-ABAD-F71582CE130E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8205"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codext - Matriz de transición" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <customWorkbookViews>
+    <customWorkbookView name="Encabezado" guid="{817BAEF7-F0B5-4F57-B3D7-04F4E674B0EF}" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="2"/>
+  </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="242">
   <si>
     <t>AA</t>
   </si>
@@ -104,15 +108,6 @@
     <t>139</t>
   </si>
   <si>
-    <t>148</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>154</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -356,9 +351,6 @@
     <t>119</t>
   </si>
   <si>
-    <t>124</t>
-  </si>
-  <si>
     <t>126</t>
   </si>
   <si>
@@ -572,9 +564,6 @@
     <t>118</t>
   </si>
   <si>
-    <t>128</t>
-  </si>
-  <si>
     <t>130</t>
   </si>
   <si>
@@ -587,9 +576,6 @@
     <t>158</t>
   </si>
   <si>
-    <t>152</t>
-  </si>
-  <si>
     <t>35</t>
   </si>
   <si>
@@ -728,9 +714,6 @@
     <t>PR18</t>
   </si>
   <si>
-    <t>PE19</t>
-  </si>
-  <si>
     <t>134</t>
   </si>
   <si>
@@ -744,12 +727,39 @@
   </si>
   <si>
     <t>Equipo 7</t>
+  </si>
+  <si>
+    <t>PR05</t>
+  </si>
+  <si>
+    <t>PR19</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>170</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -759,12 +769,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -864,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -897,6 +919,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -933,7 +964,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1227,11 +1264,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CH208"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="W3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="AV11" sqref="AV11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,7 +1282,7 @@
   <sheetData>
     <row r="1" spans="1:86" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1297,146 +1337,146 @@
     </row>
     <row r="2" spans="1:86" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="AC2" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AH2" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AL2" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AM2" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="AJ2" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="AK2" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="AL2" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="AM2" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="AN2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="AO2" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="AP2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="AQ2" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AR2" s="5" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AS2" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AT2" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="AU2" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="AV2" s="5" t="s">
-        <v>231</v>
+        <v>226</v>
+      </c>
+      <c r="AV2" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="AW2" s="5" t="s">
         <v>6</v>
@@ -1445,106 +1485,106 @@
         <v>10</v>
       </c>
       <c r="AY2" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="AZ2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="BA2" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="BB2" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="BC2" s="5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="BD2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="BE2" s="6" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="BF2" s="5" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="BG2" s="8" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="BH2" s="8" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="BI2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="BJ2" s="8" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="BK2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="BL2" s="8" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="BM2" s="8" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="BN2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="BO2" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="BP2" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="BQ2" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="BR2" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="BS2" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="BT2" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="BU2" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="BP2" s="8" t="s">
+      <c r="BV2" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="BQ2" s="8" t="s">
+      <c r="BW2" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="BR2" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="BS2" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="BT2" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="BU2" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="BV2" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="BW2" s="8" t="s">
-        <v>222</v>
       </c>
       <c r="BX2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="BY2" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="BZ2" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="CA2" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="CB2" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="CC2" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="CD2" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="CE2" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="BZ2" s="8" t="s">
+      <c r="CF2" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="CA2" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="CB2" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="CC2" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="CD2" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="CE2" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="CF2" s="8" t="s">
-        <v>230</v>
       </c>
       <c r="CG2" s="8" t="s">
         <v>13</v>
@@ -1555,17 +1595,17 @@
     </row>
     <row r="3" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B3" s="7">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>179</v>
+      <c r="C3" s="12" t="s">
+        <v>175</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="1"/>
@@ -1575,122 +1615,122 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
-        <v>180</v>
+      <c r="N3" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="O3" s="1"/>
-      <c r="P3" s="1" t="s">
-        <v>91</v>
+      <c r="P3" s="12" t="s">
+        <v>88</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="12" t="s">
         <v>19</v>
       </c>
       <c r="S3" s="1"/>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="12" t="s">
         <v>23</v>
       </c>
       <c r="U3" s="1"/>
-      <c r="V3" s="1" t="s">
-        <v>75</v>
+      <c r="V3" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="W3" s="1"/>
-      <c r="X3" s="1" t="s">
-        <v>181</v>
+      <c r="X3" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
-      <c r="AC3" s="1" t="s">
+      <c r="AC3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AD3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AE3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AF3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AG3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AH3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AI3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AJ3" s="1" t="s">
+      <c r="AJ3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AK3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AL3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AM3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AR3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AS3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AT3" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AU3" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AW3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AX3" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="AY3" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AZ3" s="3">
-        <v>132</v>
-      </c>
-      <c r="BA3" s="3">
-        <v>134</v>
-      </c>
-      <c r="BB3" s="3">
-        <v>136</v>
-      </c>
-      <c r="BC3" s="3">
-        <v>138</v>
-      </c>
-      <c r="BD3" s="3">
+      <c r="AM3" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="AN3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO3" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP3" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="AQ3" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="AR3" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="AS3" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="AT3" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="AU3" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="AV3" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="AW3" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AX3" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="AY3" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="AZ3" s="13">
+        <v>140</v>
+      </c>
+      <c r="BA3" s="13">
+        <v>142</v>
+      </c>
+      <c r="BB3" s="13">
         <v>144</v>
       </c>
-      <c r="BE3" s="3">
+      <c r="BC3" s="13">
+        <v>146</v>
+      </c>
+      <c r="BD3" s="13">
+        <v>152</v>
+      </c>
+      <c r="BE3" s="13">
         <v>41</v>
       </c>
-      <c r="BF3" s="3">
-        <v>140</v>
+      <c r="BF3" s="13">
+        <v>148</v>
       </c>
       <c r="BG3" s="3"/>
       <c r="BH3" s="3"/>
@@ -1719,7 +1759,7 @@
     </row>
     <row r="4" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B4" s="2">
         <v>1</v>
@@ -1728,8 +1768,8 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>43</v>
+      <c r="G4" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1740,8 +1780,8 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1" t="s">
-        <v>29</v>
+      <c r="Q4" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1815,8 +1855,8 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>33</v>
+      <c r="E5" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1936,8 +1976,8 @@
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
-      <c r="AM6" s="1" t="s">
-        <v>34</v>
+      <c r="AM6" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
@@ -1991,7 +2031,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="12" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="1"/>
@@ -2007,8 +2047,8 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-      <c r="U7" s="1" t="s">
-        <v>35</v>
+      <c r="U7" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -2095,8 +2135,8 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="1" t="s">
-        <v>36</v>
+      <c r="V8" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -2163,8 +2203,8 @@
       <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>37</v>
+      <c r="C9" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -2267,8 +2307,8 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="1" t="s">
-        <v>38</v>
+      <c r="T10" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
@@ -2356,8 +2396,8 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="1" t="s">
-        <v>39</v>
+      <c r="V11" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
@@ -2501,7 +2541,7 @@
       <c r="CB12" s="3"/>
       <c r="CC12" s="3"/>
       <c r="CD12" s="3"/>
-      <c r="CG12" s="3">
+      <c r="CG12" s="13">
         <v>10</v>
       </c>
       <c r="CH12" s="3"/>
@@ -2589,8 +2629,8 @@
       <c r="CC13" s="3"/>
       <c r="CD13" s="3"/>
       <c r="CG13" s="3"/>
-      <c r="CH13" s="3" t="s">
-        <v>40</v>
+      <c r="CH13" s="13" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:86" x14ac:dyDescent="0.25">
@@ -2610,8 +2650,8 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1" t="s">
-        <v>41</v>
+      <c r="P14" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -2687,7 +2727,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="1"/>
@@ -2851,7 +2891,7 @@
       <c r="CB16" s="3"/>
       <c r="CC16" s="3"/>
       <c r="CD16" s="3"/>
-      <c r="CG16" s="3">
+      <c r="CG16" s="13">
         <v>14</v>
       </c>
       <c r="CH16" s="3"/>
@@ -2941,8 +2981,8 @@
       <c r="CC17" s="3"/>
       <c r="CD17" s="3"/>
       <c r="CG17" s="3"/>
-      <c r="CH17" s="3" t="s">
-        <v>42</v>
+      <c r="CH17" s="13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:86" x14ac:dyDescent="0.25">
@@ -2951,7 +2991,7 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="1"/>
@@ -3043,13 +3083,13 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>190</v>
+      <c r="H19" s="12" t="s">
+        <v>184</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1" t="s">
-        <v>45</v>
+      <c r="K19" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -3132,8 +3172,8 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1" t="s">
-        <v>191</v>
+      <c r="F20" s="12" t="s">
+        <v>185</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -3222,8 +3262,8 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>192</v>
+      <c r="G21" s="12" t="s">
+        <v>186</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -3387,7 +3427,7 @@
       <c r="CB22" s="3"/>
       <c r="CC22" s="3"/>
       <c r="CD22" s="3"/>
-      <c r="CG22" s="3">
+      <c r="CG22" s="13">
         <v>20</v>
       </c>
       <c r="CH22" s="3"/>
@@ -3477,16 +3517,16 @@
       <c r="CC23" s="3"/>
       <c r="CD23" s="3"/>
       <c r="CG23" s="3"/>
-      <c r="CH23" s="3" t="s">
-        <v>53</v>
+      <c r="CH23" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>21</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>193</v>
+      <c r="C24" s="12" t="s">
+        <v>187</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -3585,8 +3625,8 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="N25" s="1" t="s">
-        <v>194</v>
+      <c r="N25" s="12" t="s">
+        <v>188</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -3681,8 +3721,8 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
-      <c r="U26" s="1" t="s">
-        <v>44</v>
+      <c r="U26" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
@@ -3756,8 +3796,8 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1" t="s">
-        <v>63</v>
+      <c r="G27" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -3921,7 +3961,7 @@
       <c r="CB28" s="3"/>
       <c r="CC28" s="3"/>
       <c r="CD28" s="3"/>
-      <c r="CG28" s="3">
+      <c r="CG28" s="13">
         <v>26</v>
       </c>
       <c r="CH28" s="3"/>
@@ -4011,8 +4051,8 @@
       <c r="CC29" s="3"/>
       <c r="CD29" s="3"/>
       <c r="CG29" s="3"/>
-      <c r="CH29" s="3" t="s">
-        <v>54</v>
+      <c r="CH29" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="2:86" x14ac:dyDescent="0.25">
@@ -4045,34 +4085,34 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
-      <c r="AC30" s="1" t="s">
+      <c r="AC30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AD30" s="1" t="s">
+      <c r="AD30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AE30" s="1" t="s">
+      <c r="AE30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AF30" s="1" t="s">
+      <c r="AF30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AG30" s="1" t="s">
+      <c r="AG30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AH30" s="1" t="s">
+      <c r="AH30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AI30" s="1" t="s">
+      <c r="AI30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AJ30" s="1" t="s">
+      <c r="AJ30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AK30" s="1" t="s">
+      <c r="AK30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AL30" s="1" t="s">
+      <c r="AL30" s="12" t="s">
         <v>18</v>
       </c>
       <c r="AM30" s="1"/>
@@ -4094,7 +4134,7 @@
       <c r="BC30" s="3"/>
       <c r="BD30" s="3"/>
       <c r="BE30" s="3"/>
-      <c r="BF30" s="3">
+      <c r="BF30" s="13">
         <v>29</v>
       </c>
       <c r="BG30" s="3"/>
@@ -4121,7 +4161,7 @@
       <c r="CB30" s="3"/>
       <c r="CC30" s="3"/>
       <c r="CD30" s="3"/>
-      <c r="CG30" s="3">
+      <c r="CG30" s="13">
         <v>28</v>
       </c>
       <c r="CH30" s="3"/>
@@ -4211,8 +4251,8 @@
       <c r="CC31" s="3"/>
       <c r="CD31" s="3"/>
       <c r="CG31" s="3"/>
-      <c r="CH31" s="3" t="s">
-        <v>195</v>
+      <c r="CH31" s="13" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="2:86" x14ac:dyDescent="0.25">
@@ -4299,7 +4339,7 @@
       <c r="CB32" s="3"/>
       <c r="CC32" s="3"/>
       <c r="CD32" s="3"/>
-      <c r="CG32" s="3">
+      <c r="CG32" s="13">
         <v>30</v>
       </c>
       <c r="CH32" s="3"/>
@@ -4389,8 +4429,8 @@
       <c r="CC33" s="3"/>
       <c r="CD33" s="3"/>
       <c r="CG33" s="3"/>
-      <c r="CH33" s="3" t="s">
-        <v>46</v>
+      <c r="CH33" s="13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="2:86" x14ac:dyDescent="0.25">
@@ -4401,7 +4441,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="12" t="s">
         <v>15</v>
       </c>
       <c r="H34" s="1"/>
@@ -4425,43 +4465,43 @@
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
-      <c r="AC34" s="1" t="s">
+      <c r="AC34" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AD34" s="1" t="s">
+      <c r="AD34" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AE34" s="1" t="s">
+      <c r="AE34" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AF34" s="1" t="s">
+      <c r="AF34" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AG34" s="1" t="s">
+      <c r="AG34" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AH34" s="1" t="s">
+      <c r="AH34" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AI34" s="1" t="s">
+      <c r="AI34" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AJ34" s="1" t="s">
+      <c r="AJ34" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AK34" s="1" t="s">
+      <c r="AK34" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AL34" s="1" t="s">
+      <c r="AL34" s="12" t="s">
         <v>18</v>
       </c>
       <c r="AM34" s="1"/>
       <c r="AN34" s="1"/>
-      <c r="AO34" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP34" s="1" t="s">
-        <v>196</v>
+      <c r="AO34" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP34" s="12" t="s">
+        <v>190</v>
       </c>
       <c r="AQ34" s="1"/>
       <c r="AR34" s="1"/>
@@ -4536,34 +4576,34 @@
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
       <c r="AB35" s="1"/>
-      <c r="AC35" s="1" t="s">
+      <c r="AC35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AD35" s="1" t="s">
+      <c r="AD35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AE35" s="1" t="s">
+      <c r="AE35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AF35" s="1" t="s">
+      <c r="AF35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AG35" s="1" t="s">
+      <c r="AG35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AH35" s="1" t="s">
+      <c r="AH35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AI35" s="1" t="s">
+      <c r="AI35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AJ35" s="1" t="s">
+      <c r="AJ35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AK35" s="1" t="s">
+      <c r="AK35" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AL35" s="1" t="s">
+      <c r="AL35" s="12" t="s">
         <v>22</v>
       </c>
       <c r="AM35" s="1"/>
@@ -4621,7 +4661,7 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="12" t="s">
         <v>15</v>
       </c>
       <c r="H36" s="1"/>
@@ -4645,40 +4685,40 @@
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
-      <c r="AC36" s="1" t="s">
+      <c r="AC36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AD36" s="1" t="s">
+      <c r="AD36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AE36" s="1" t="s">
+      <c r="AE36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AF36" s="1" t="s">
+      <c r="AF36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AG36" s="1" t="s">
+      <c r="AG36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AH36" s="1" t="s">
+      <c r="AH36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AI36" s="1" t="s">
+      <c r="AI36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AJ36" s="1" t="s">
+      <c r="AJ36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AK36" s="1" t="s">
+      <c r="AK36" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="AL36" s="1" t="s">
+      <c r="AL36" s="12" t="s">
         <v>22</v>
       </c>
       <c r="AM36" s="1"/>
       <c r="AN36" s="1"/>
-      <c r="AO36" s="1" t="s">
-        <v>65</v>
+      <c r="AO36" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="AP36" s="1"/>
       <c r="AQ36" s="1"/>
@@ -4765,8 +4805,8 @@
       <c r="AK37" s="1"/>
       <c r="AL37" s="1"/>
       <c r="AM37" s="1"/>
-      <c r="AN37" s="1" t="s">
-        <v>188</v>
+      <c r="AN37" s="12" t="s">
+        <v>182</v>
       </c>
       <c r="AO37" s="1"/>
       <c r="AP37" s="1"/>
@@ -4776,8 +4816,8 @@
       <c r="AT37" s="1"/>
       <c r="AU37" s="1"/>
       <c r="AV37" s="1"/>
-      <c r="AW37" s="1" t="s">
-        <v>188</v>
+      <c r="AW37" s="12" t="s">
+        <v>182</v>
       </c>
       <c r="AX37" s="1"/>
       <c r="AY37" s="1"/>
@@ -4845,35 +4885,35 @@
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
       <c r="AB38" s="1"/>
-      <c r="AC38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL38" s="1" t="s">
-        <v>66</v>
+      <c r="AC38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK38" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL38" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="AM38" s="1"/>
       <c r="AN38" s="1"/>
@@ -4952,40 +4992,40 @@
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
       <c r="AB39" s="1"/>
-      <c r="AC39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AE39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AK39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AL39" s="1" t="s">
-        <v>66</v>
+      <c r="AC39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL39" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="AM39" s="1"/>
       <c r="AN39" s="1"/>
-      <c r="AO39" s="1" t="s">
-        <v>65</v>
+      <c r="AO39" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="AP39" s="1"/>
       <c r="AQ39" s="1"/>
@@ -5115,7 +5155,7 @@
       <c r="CB40" s="3"/>
       <c r="CC40" s="3"/>
       <c r="CD40" s="3"/>
-      <c r="CG40" s="3">
+      <c r="CG40" s="13">
         <v>38</v>
       </c>
       <c r="CH40" s="3"/>
@@ -5205,8 +5245,8 @@
       <c r="CC41" s="3"/>
       <c r="CD41" s="3"/>
       <c r="CG41" s="3"/>
-      <c r="CH41" s="3" t="s">
-        <v>197</v>
+      <c r="CH41" s="13" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="2:86" x14ac:dyDescent="0.25">
@@ -5293,7 +5333,7 @@
       <c r="CB42" s="3"/>
       <c r="CC42" s="3"/>
       <c r="CD42" s="3"/>
-      <c r="CG42" s="3">
+      <c r="CG42" s="13">
         <v>40</v>
       </c>
       <c r="CH42" s="3"/>
@@ -5383,8 +5423,8 @@
       <c r="CC43" s="3"/>
       <c r="CD43" s="3"/>
       <c r="CG43" s="3"/>
-      <c r="CH43" s="3" t="s">
-        <v>68</v>
+      <c r="CH43" s="13" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="2:86" x14ac:dyDescent="0.25">
@@ -5428,25 +5468,25 @@
       <c r="AK44" s="1"/>
       <c r="AL44" s="1"/>
       <c r="AM44" s="1"/>
-      <c r="AN44" s="1" t="s">
-        <v>30</v>
+      <c r="AN44" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="AO44" s="1"/>
       <c r="AP44" s="1"/>
       <c r="AQ44" s="1"/>
-      <c r="AR44" s="1" t="s">
-        <v>69</v>
+      <c r="AR44" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="AS44" s="1"/>
       <c r="AT44" s="1"/>
       <c r="AU44" s="1"/>
       <c r="AV44" s="1"/>
       <c r="AW44" s="1"/>
-      <c r="AX44" s="1" t="s">
-        <v>31</v>
+      <c r="AX44" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="AY44" s="1"/>
-      <c r="AZ44" s="3">
+      <c r="AZ44" s="13">
         <v>47</v>
       </c>
       <c r="BA44" s="3"/>
@@ -5454,7 +5494,7 @@
       <c r="BC44" s="3"/>
       <c r="BD44" s="3"/>
       <c r="BE44" s="3"/>
-      <c r="BF44" s="3">
+      <c r="BF44" s="13">
         <v>45</v>
       </c>
       <c r="BG44" s="3"/>
@@ -5481,7 +5521,7 @@
       <c r="CB44" s="3"/>
       <c r="CC44" s="3"/>
       <c r="CD44" s="3"/>
-      <c r="CG44" s="3">
+      <c r="CG44" s="13">
         <v>42</v>
       </c>
       <c r="CH44" s="3"/>
@@ -5571,8 +5611,8 @@
       <c r="CC45" s="3"/>
       <c r="CD45" s="3"/>
       <c r="CG45" s="3"/>
-      <c r="CH45" s="3" t="s">
-        <v>70</v>
+      <c r="CH45" s="13" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="2:86" x14ac:dyDescent="0.25">
@@ -5659,7 +5699,7 @@
       <c r="CB46" s="3"/>
       <c r="CC46" s="3"/>
       <c r="CD46" s="3"/>
-      <c r="CG46" s="3">
+      <c r="CG46" s="13">
         <v>44</v>
       </c>
       <c r="CH46" s="3"/>
@@ -5749,8 +5789,8 @@
       <c r="CC47" s="3"/>
       <c r="CD47" s="3"/>
       <c r="CG47" s="3"/>
-      <c r="CH47" s="3" t="s">
-        <v>47</v>
+      <c r="CH47" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="2:86" x14ac:dyDescent="0.25">
@@ -5837,7 +5877,7 @@
       <c r="CB48" s="3"/>
       <c r="CC48" s="3"/>
       <c r="CD48" s="3"/>
-      <c r="CG48" s="3">
+      <c r="CG48" s="13">
         <v>46</v>
       </c>
       <c r="CH48" s="3"/>
@@ -5927,8 +5967,8 @@
       <c r="CC49" s="3"/>
       <c r="CD49" s="3"/>
       <c r="CG49" s="3"/>
-      <c r="CH49" s="3" t="s">
-        <v>71</v>
+      <c r="CH49" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="2:86" x14ac:dyDescent="0.25">
@@ -6015,7 +6055,7 @@
       <c r="CB50" s="3"/>
       <c r="CC50" s="3"/>
       <c r="CD50" s="3"/>
-      <c r="CG50" s="3">
+      <c r="CG50" s="13">
         <v>48</v>
       </c>
       <c r="CH50" s="3"/>
@@ -6105,259 +6145,259 @@
       <c r="CC51" s="3"/>
       <c r="CD51" s="3"/>
       <c r="CG51" s="3"/>
-      <c r="CH51" s="3" t="s">
-        <v>72</v>
+      <c r="CH51" s="13" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
         <v>49</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="R52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="S52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="T52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="U52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="W52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="X52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AJ52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AM52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AQ52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AR52" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AT52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AU52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AV52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AW52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AX52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AZ52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BA52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BB52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BC52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BD52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BE52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BF52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BG52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BH52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BI52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BJ52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BK52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BL52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BM52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BN52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BO52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BP52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BQ52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BR52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BT52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BU52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BV52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BW52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BX52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BY52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BZ52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="CA52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="CB52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="CC52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="CD52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="CE52" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="CF52" s="1" t="s">
-        <v>69</v>
+      <c r="C52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="L52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="N52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="O52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="P52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="R52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="S52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="T52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="U52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="V52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="W52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="X52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR52" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AU52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AW52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AX52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AZ52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BA52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BC52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BE52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BF52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BG52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BH52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BI52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BJ52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BK52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BL52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BO52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BR52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BS52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BT52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BU52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BV52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BW52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BX52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BY52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BZ52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CA52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CB52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CC52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CD52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CE52" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="CF52" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="CG52" s="3"/>
       <c r="CH52" s="3"/>
@@ -6421,7 +6461,7 @@
       <c r="BC53" s="3"/>
       <c r="BD53" s="3"/>
       <c r="BE53" s="3"/>
-      <c r="BF53" s="3">
+      <c r="BF53" s="13">
         <v>51</v>
       </c>
       <c r="BG53" s="3"/>
@@ -6535,7 +6575,7 @@
       <c r="CB54" s="3"/>
       <c r="CC54" s="3"/>
       <c r="CD54" s="3"/>
-      <c r="CG54" s="3">
+      <c r="CG54" s="13">
         <v>52</v>
       </c>
       <c r="CH54" s="3"/>
@@ -6625,259 +6665,259 @@
       <c r="CC55" s="3"/>
       <c r="CD55" s="3"/>
       <c r="CG55" s="3"/>
-      <c r="CH55" s="3" t="s">
-        <v>62</v>
+      <c r="CH55" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
         <v>53</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="R56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="U56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="W56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AO56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AQ56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AR56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AS56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AT56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AU56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AV56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AW56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AX56" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AY56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AZ56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BA56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BB56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BC56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BD56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BE56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BF56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BG56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BH56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BI56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BJ56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BK56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BL56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BM56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BN56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BO56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BP56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BQ56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BR56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BS56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BT56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BU56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BV56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BW56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BX56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BY56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BZ56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CA56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CB56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CC56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CD56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CE56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CF56" s="1" t="s">
-        <v>31</v>
+      <c r="C56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="T56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="U56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="V56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="X56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AP56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AT56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AU56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AV56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AW56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AX56" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BA56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BB56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BC56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BD56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BE56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BF56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BG56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BH56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BI56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BJ56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BK56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BL56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BM56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BN56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BO56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BP56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BQ56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BR56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BS56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BT56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BU56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BV56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BW56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BX56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BY56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BZ56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="CA56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="CB56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="CC56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="CD56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="CE56" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="CF56" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="CG56" s="3"/>
       <c r="CH56" s="3"/>
@@ -6941,7 +6981,7 @@
       <c r="BC57" s="3"/>
       <c r="BD57" s="3"/>
       <c r="BE57" s="3"/>
-      <c r="BF57" s="3">
+      <c r="BF57" s="13">
         <v>55</v>
       </c>
       <c r="BG57" s="3"/>
@@ -7055,7 +7095,7 @@
       <c r="CB58" s="3"/>
       <c r="CC58" s="3"/>
       <c r="CD58" s="3"/>
-      <c r="CG58" s="3">
+      <c r="CG58" s="13">
         <v>56</v>
       </c>
       <c r="CH58" s="3"/>
@@ -7145,16 +7185,16 @@
       <c r="CC59" s="3"/>
       <c r="CD59" s="3"/>
       <c r="CG59" s="3"/>
-      <c r="CH59" s="3" t="s">
-        <v>61</v>
+      <c r="CH59" s="13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
         <v>57</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>201</v>
+      <c r="C60" s="12" t="s">
+        <v>195</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -7163,8 +7203,8 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="1" t="s">
-        <v>198</v>
+      <c r="K60" s="12" t="s">
+        <v>192</v>
       </c>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
@@ -7255,11 +7295,11 @@
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
-      <c r="N61" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O61" s="1" t="s">
-        <v>76</v>
+      <c r="N61" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="O61" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
@@ -7267,8 +7307,8 @@
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
-      <c r="V61" s="1" t="s">
-        <v>199</v>
+      <c r="V61" s="12" t="s">
+        <v>193</v>
       </c>
       <c r="W61" s="1"/>
       <c r="X61" s="1"/>
@@ -7348,8 +7388,8 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
-      <c r="N62" s="1" t="s">
-        <v>200</v>
+      <c r="N62" s="12" t="s">
+        <v>194</v>
       </c>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
@@ -7430,7 +7470,7 @@
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-      <c r="G63" s="1" t="s">
+      <c r="G63" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H63" s="1"/>
@@ -7595,7 +7635,7 @@
       <c r="CB64" s="3"/>
       <c r="CC64" s="3"/>
       <c r="CD64" s="3"/>
-      <c r="CG64" s="3">
+      <c r="CG64" s="13">
         <v>62</v>
       </c>
       <c r="CH64" s="3"/>
@@ -7685,8 +7725,8 @@
       <c r="CC65" s="3"/>
       <c r="CD65" s="3"/>
       <c r="CG65" s="3"/>
-      <c r="CH65" s="3" t="s">
-        <v>58</v>
+      <c r="CH65" s="13" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="66" spans="2:86" x14ac:dyDescent="0.25">
@@ -7773,7 +7813,7 @@
       <c r="CB66" s="3"/>
       <c r="CC66" s="3"/>
       <c r="CD66" s="3"/>
-      <c r="CG66" s="3">
+      <c r="CG66" s="13">
         <v>64</v>
       </c>
       <c r="CH66" s="3"/>
@@ -7863,8 +7903,8 @@
       <c r="CC67" s="3"/>
       <c r="CD67" s="3"/>
       <c r="CG67" s="3"/>
-      <c r="CH67" s="3" t="s">
-        <v>57</v>
+      <c r="CH67" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="2:86" x14ac:dyDescent="0.25">
@@ -7875,8 +7915,8 @@
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-      <c r="G68" s="1" t="s">
-        <v>77</v>
+      <c r="G68" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
@@ -7978,8 +8018,8 @@
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
-      <c r="U69" s="1" t="s">
-        <v>78</v>
+      <c r="U69" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
@@ -8129,7 +8169,7 @@
       <c r="CB70" s="3"/>
       <c r="CC70" s="3"/>
       <c r="CD70" s="3"/>
-      <c r="CG70" s="3">
+      <c r="CG70" s="13">
         <v>68</v>
       </c>
       <c r="CH70" s="3"/>
@@ -8219,8 +8259,8 @@
       <c r="CC71" s="3"/>
       <c r="CD71" s="3"/>
       <c r="CG71" s="3"/>
-      <c r="CH71" s="3" t="s">
-        <v>58</v>
+      <c r="CH71" s="13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="2:86" x14ac:dyDescent="0.25">
@@ -8228,8 +8268,8 @@
         <v>69</v>
       </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="1" t="s">
-        <v>202</v>
+      <c r="D72" s="12" t="s">
+        <v>196</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -8327,8 +8367,8 @@
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
-      <c r="N73" s="1" t="s">
-        <v>79</v>
+      <c r="N73" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
@@ -8409,8 +8449,8 @@
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="1" t="s">
-        <v>80</v>
+      <c r="G74" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
@@ -8530,8 +8570,8 @@
       <c r="AJ75" s="1"/>
       <c r="AK75" s="1"/>
       <c r="AL75" s="1"/>
-      <c r="AM75" s="1" t="s">
-        <v>81</v>
+      <c r="AM75" s="12" t="s">
+        <v>78</v>
       </c>
       <c r="AN75" s="1"/>
       <c r="AO75" s="1"/>
@@ -8576,7 +8616,7 @@
       <c r="CB75" s="3"/>
       <c r="CC75" s="3"/>
       <c r="CD75" s="3"/>
-      <c r="CG75" s="3">
+      <c r="CG75" s="13">
         <v>73</v>
       </c>
       <c r="CH75" s="3"/>
@@ -8666,8 +8706,8 @@
       <c r="CC76" s="3"/>
       <c r="CD76" s="3"/>
       <c r="CG76" s="3"/>
-      <c r="CH76" s="3" t="s">
-        <v>51</v>
+      <c r="CH76" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="77" spans="2:86" x14ac:dyDescent="0.25">
@@ -8691,8 +8731,8 @@
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
       <c r="S77" s="1"/>
-      <c r="T77" s="1" t="s">
-        <v>189</v>
+      <c r="T77" s="12" t="s">
+        <v>183</v>
       </c>
       <c r="U77" s="1"/>
       <c r="V77" s="1"/>
@@ -8777,8 +8817,8 @@
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
-      <c r="Q78" s="1" t="s">
-        <v>82</v>
+      <c r="Q78" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="R78" s="1"/>
       <c r="S78" s="1"/>
@@ -8874,8 +8914,8 @@
       <c r="V79" s="1"/>
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
-      <c r="Y79" s="1" t="s">
-        <v>203</v>
+      <c r="Y79" s="12" t="s">
+        <v>197</v>
       </c>
       <c r="Z79" s="1"/>
       <c r="AA79" s="1"/>
@@ -9021,7 +9061,7 @@
       <c r="CB80" s="3"/>
       <c r="CC80" s="3"/>
       <c r="CD80" s="3"/>
-      <c r="CG80" s="3">
+      <c r="CG80" s="13">
         <v>78</v>
       </c>
       <c r="CH80" s="3"/>
@@ -9111,16 +9151,16 @@
       <c r="CC81" s="3"/>
       <c r="CD81" s="3"/>
       <c r="CG81" s="3"/>
-      <c r="CH81" s="3" t="s">
-        <v>52</v>
+      <c r="CH81" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="82" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>83</v>
+      <c r="C82" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -9214,8 +9254,8 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
-      <c r="I83" s="1" t="s">
-        <v>84</v>
+      <c r="I83" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
@@ -9301,8 +9341,8 @@
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-      <c r="G84" s="1" t="s">
-        <v>85</v>
+      <c r="G84" s="12" t="s">
+        <v>82</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
@@ -9422,8 +9462,8 @@
       <c r="AJ85" s="1"/>
       <c r="AK85" s="1"/>
       <c r="AL85" s="1"/>
-      <c r="AM85" s="1" t="s">
-        <v>86</v>
+      <c r="AM85" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="AN85" s="1"/>
       <c r="AO85" s="1"/>
@@ -9484,8 +9524,8 @@
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
-      <c r="L86" s="1" t="s">
-        <v>87</v>
+      <c r="L86" s="12" t="s">
+        <v>84</v>
       </c>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
@@ -9584,8 +9624,8 @@
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
       <c r="V87" s="1"/>
-      <c r="W87" s="1" t="s">
-        <v>88</v>
+      <c r="W87" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="X87" s="1"/>
       <c r="Y87" s="1"/>
@@ -9665,8 +9705,8 @@
       <c r="L88" s="1"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
-      <c r="O88" s="1" t="s">
-        <v>89</v>
+      <c r="O88" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
@@ -9757,8 +9797,8 @@
       <c r="O89" s="1"/>
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
-      <c r="R89" s="1" t="s">
-        <v>90</v>
+      <c r="R89" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="S89" s="1"/>
       <c r="T89" s="1"/>
@@ -9911,7 +9951,7 @@
       <c r="CB90" s="3"/>
       <c r="CC90" s="3"/>
       <c r="CD90" s="3"/>
-      <c r="CG90" s="3">
+      <c r="CG90" s="13">
         <v>88</v>
       </c>
       <c r="CH90" s="3"/>
@@ -10001,8 +10041,8 @@
       <c r="CC91" s="3"/>
       <c r="CD91" s="3"/>
       <c r="CG91" s="3"/>
-      <c r="CH91" s="3" t="s">
-        <v>48</v>
+      <c r="CH91" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="92" spans="2:86" x14ac:dyDescent="0.25">
@@ -10013,8 +10053,8 @@
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
-      <c r="G92" s="1" t="s">
-        <v>92</v>
+      <c r="G92" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
@@ -10121,8 +10161,8 @@
       <c r="W93" s="1"/>
       <c r="X93" s="1"/>
       <c r="Y93" s="1"/>
-      <c r="Z93" s="1" t="s">
-        <v>93</v>
+      <c r="Z93" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="AA93" s="1"/>
       <c r="AB93" s="1"/>
@@ -10206,8 +10246,8 @@
       <c r="S94" s="1"/>
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
-      <c r="V94" s="1" t="s">
-        <v>94</v>
+      <c r="V94" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="W94" s="1"/>
       <c r="X94" s="1"/>
@@ -10312,8 +10352,8 @@
       <c r="AJ95" s="1"/>
       <c r="AK95" s="1"/>
       <c r="AL95" s="1"/>
-      <c r="AM95" s="1" t="s">
-        <v>95</v>
+      <c r="AM95" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="AN95" s="1"/>
       <c r="AO95" s="1"/>
@@ -10376,8 +10416,8 @@
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
       <c r="M96" s="1"/>
-      <c r="N96" s="1" t="s">
-        <v>96</v>
+      <c r="N96" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="O96" s="1"/>
       <c r="P96" s="1"/>
@@ -10462,8 +10502,8 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
-      <c r="K97" s="1" t="s">
-        <v>97</v>
+      <c r="K97" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="L97" s="1"/>
       <c r="M97" s="1"/>
@@ -10556,8 +10596,8 @@
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
-      <c r="P98" s="1" t="s">
-        <v>98</v>
+      <c r="P98" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="Q98" s="1"/>
       <c r="R98" s="1"/>
@@ -10636,8 +10676,8 @@
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
-      <c r="G99" s="1" t="s">
-        <v>204</v>
+      <c r="G99" s="12" t="s">
+        <v>198</v>
       </c>
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
@@ -10801,7 +10841,7 @@
       <c r="CB100" s="3"/>
       <c r="CC100" s="3"/>
       <c r="CD100" s="3"/>
-      <c r="CG100" s="3">
+      <c r="CG100" s="13">
         <v>98</v>
       </c>
       <c r="CH100" s="3"/>
@@ -10891,8 +10931,8 @@
       <c r="CC101" s="3"/>
       <c r="CD101" s="3"/>
       <c r="CG101" s="3"/>
-      <c r="CH101" s="3" t="s">
-        <v>49</v>
+      <c r="CH101" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="102" spans="2:86" x14ac:dyDescent="0.25">
@@ -10916,7 +10956,7 @@
       <c r="Q102" s="1"/>
       <c r="R102" s="1"/>
       <c r="S102" s="1"/>
-      <c r="T102" s="1" t="s">
+      <c r="T102" s="12" t="s">
         <v>20</v>
       </c>
       <c r="U102" s="1"/>
@@ -10996,8 +11036,8 @@
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
-      <c r="K103" s="1" t="s">
-        <v>99</v>
+      <c r="K103" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
@@ -11096,8 +11136,8 @@
       <c r="S104" s="1"/>
       <c r="T104" s="1"/>
       <c r="U104" s="1"/>
-      <c r="V104" s="1" t="s">
-        <v>100</v>
+      <c r="V104" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="W104" s="1"/>
       <c r="X104" s="1"/>
@@ -11173,8 +11213,8 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
       <c r="I105" s="1"/>
-      <c r="J105" s="1" t="s">
-        <v>101</v>
+      <c r="J105" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
@@ -11335,7 +11375,7 @@
       <c r="CB106" s="3"/>
       <c r="CC106" s="3"/>
       <c r="CD106" s="3"/>
-      <c r="CG106" s="3">
+      <c r="CG106" s="13">
         <v>104</v>
       </c>
       <c r="CH106" s="3"/>
@@ -11425,8 +11465,8 @@
       <c r="CC107" s="3"/>
       <c r="CD107" s="3"/>
       <c r="CG107" s="3"/>
-      <c r="CH107" s="3" t="s">
-        <v>50</v>
+      <c r="CH107" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="108" spans="2:86" x14ac:dyDescent="0.25">
@@ -11447,8 +11487,8 @@
       <c r="N108" s="1"/>
       <c r="O108" s="1"/>
       <c r="P108" s="1"/>
-      <c r="Q108" s="1" t="s">
-        <v>102</v>
+      <c r="Q108" s="12" t="s">
+        <v>99</v>
       </c>
       <c r="R108" s="1"/>
       <c r="S108" s="1"/>
@@ -11528,8 +11568,8 @@
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
-      <c r="I109" s="1" t="s">
-        <v>103</v>
+      <c r="I109" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
@@ -11619,8 +11659,8 @@
       <c r="H110" s="1"/>
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
-      <c r="K110" s="1" t="s">
-        <v>205</v>
+      <c r="K110" s="12" t="s">
+        <v>199</v>
       </c>
       <c r="L110" s="1"/>
       <c r="M110" s="1"/>
@@ -11702,8 +11742,8 @@
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
-      <c r="E111" s="1" t="s">
-        <v>104</v>
+      <c r="E111" s="12" t="s">
+        <v>101</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
@@ -11869,7 +11909,7 @@
       <c r="CB112" s="3"/>
       <c r="CC112" s="3"/>
       <c r="CD112" s="3"/>
-      <c r="CG112" s="3">
+      <c r="CG112" s="13">
         <v>110</v>
       </c>
       <c r="CH112" s="3"/>
@@ -11959,8 +11999,8 @@
       <c r="CC113" s="3"/>
       <c r="CD113" s="3"/>
       <c r="CG113" s="3"/>
-      <c r="CH113" s="3" t="s">
-        <v>55</v>
+      <c r="CH113" s="13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="114" spans="2:86" x14ac:dyDescent="0.25">
@@ -11971,8 +12011,8 @@
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
-      <c r="G114" s="1" t="s">
-        <v>105</v>
+      <c r="G114" s="12" t="s">
+        <v>102</v>
       </c>
       <c r="H114" s="1"/>
       <c r="I114" s="1"/>
@@ -12071,8 +12111,8 @@
       <c r="O115" s="1"/>
       <c r="P115" s="1"/>
       <c r="Q115" s="1"/>
-      <c r="R115" s="1" t="s">
-        <v>106</v>
+      <c r="R115" s="12" t="s">
+        <v>103</v>
       </c>
       <c r="S115" s="1"/>
       <c r="T115" s="1"/>
@@ -12149,8 +12189,8 @@
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
-      <c r="G116" s="1" t="s">
-        <v>107</v>
+      <c r="G116" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="H116" s="1"/>
       <c r="I116" s="1"/>
@@ -12234,8 +12274,8 @@
       <c r="B117" s="2">
         <v>114</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>108</v>
+      <c r="C117" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
@@ -12342,8 +12382,8 @@
       <c r="S118" s="1"/>
       <c r="T118" s="1"/>
       <c r="U118" s="1"/>
-      <c r="V118" s="1" t="s">
-        <v>206</v>
+      <c r="V118" s="12" t="s">
+        <v>200</v>
       </c>
       <c r="W118" s="1"/>
       <c r="X118" s="1"/>
@@ -12492,7 +12532,7 @@
       <c r="CB119" s="3"/>
       <c r="CC119" s="3"/>
       <c r="CD119" s="3"/>
-      <c r="CG119" s="3">
+      <c r="CG119" s="13">
         <v>117</v>
       </c>
       <c r="CH119" s="3"/>
@@ -12582,16 +12622,16 @@
       <c r="CC120" s="3"/>
       <c r="CD120" s="3"/>
       <c r="CG120" s="3"/>
-      <c r="CH120" s="3" t="s">
-        <v>56</v>
+      <c r="CH120" s="13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="121" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B121" s="2">
         <v>118</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>109</v>
+      <c r="C121" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
@@ -12600,8 +12640,8 @@
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="1"/>
-      <c r="K121" s="1" t="s">
-        <v>111</v>
+      <c r="K121" s="12" t="s">
+        <v>107</v>
       </c>
       <c r="L121" s="1"/>
       <c r="M121" s="1"/>
@@ -12692,7 +12732,7 @@
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
       <c r="M122" s="1"/>
-      <c r="N122" s="1" t="s">
+      <c r="N122" s="12" t="s">
         <v>24</v>
       </c>
       <c r="O122" s="1"/>
@@ -12700,8 +12740,8 @@
       <c r="Q122" s="1"/>
       <c r="R122" s="1"/>
       <c r="S122" s="1"/>
-      <c r="T122" s="1" t="s">
-        <v>207</v>
+      <c r="T122" s="12" t="s">
+        <v>201</v>
       </c>
       <c r="U122" s="1"/>
       <c r="V122" s="1"/>
@@ -12852,7 +12892,7 @@
       <c r="CB123" s="3"/>
       <c r="CC123" s="3"/>
       <c r="CD123" s="3"/>
-      <c r="CG123" s="3">
+      <c r="CG123" s="13">
         <v>121</v>
       </c>
       <c r="CH123" s="3"/>
@@ -12942,8 +12982,8 @@
       <c r="CC124" s="3"/>
       <c r="CD124" s="3"/>
       <c r="CG124" s="3"/>
-      <c r="CH124" s="3" t="s">
-        <v>59</v>
+      <c r="CH124" s="13" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="125" spans="2:86" x14ac:dyDescent="0.25">
@@ -12970,7 +13010,7 @@
       <c r="T125" s="3"/>
       <c r="U125" s="3"/>
       <c r="V125" s="3"/>
-      <c r="W125" s="3">
+      <c r="W125" s="13">
         <v>123</v>
       </c>
       <c r="X125" s="3"/>
@@ -13045,7 +13085,7 @@
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
-      <c r="G126" s="3">
+      <c r="G126" s="13">
         <v>124</v>
       </c>
       <c r="H126" s="3"/>
@@ -13214,7 +13254,7 @@
       <c r="CD127" s="3"/>
       <c r="CE127" s="3"/>
       <c r="CF127" s="3"/>
-      <c r="CG127" s="3">
+      <c r="CG127" s="13">
         <v>125</v>
       </c>
       <c r="CH127" s="3"/>
@@ -13306,8 +13346,8 @@
       <c r="CE128" s="3"/>
       <c r="CF128" s="3"/>
       <c r="CG128" s="3"/>
-      <c r="CH128" s="3" t="s">
-        <v>233</v>
+      <c r="CH128" s="13" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="129" spans="2:86" x14ac:dyDescent="0.25">
@@ -13318,7 +13358,7 @@
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
-      <c r="G129" s="3">
+      <c r="G129" s="13">
         <v>127</v>
       </c>
       <c r="H129" s="3"/>
@@ -13427,7 +13467,7 @@
       <c r="V130" s="3"/>
       <c r="W130" s="3"/>
       <c r="X130" s="3"/>
-      <c r="Y130" s="3">
+      <c r="Y130" s="13">
         <v>128</v>
       </c>
       <c r="Z130" s="3"/>
@@ -13578,7 +13618,7 @@
       <c r="CD131" s="3"/>
       <c r="CE131" s="3"/>
       <c r="CF131" s="3"/>
-      <c r="CG131" s="3">
+      <c r="CG131" s="13">
         <v>129</v>
       </c>
       <c r="CH131" s="3"/>
@@ -13670,7 +13710,7 @@
       <c r="CE132" s="3"/>
       <c r="CF132" s="3"/>
       <c r="CG132" s="3"/>
-      <c r="CH132" s="3" t="s">
+      <c r="CH132" s="13" t="s">
         <v>234</v>
       </c>
     </row>
@@ -13704,34 +13744,34 @@
       <c r="Z133" s="1"/>
       <c r="AA133" s="1"/>
       <c r="AB133" s="1"/>
-      <c r="AC133" s="1" t="s">
+      <c r="AC133" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AD133" s="1" t="s">
+      <c r="AD133" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AE133" s="1" t="s">
+      <c r="AE133" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AF133" s="1" t="s">
+      <c r="AF133" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AG133" s="1" t="s">
+      <c r="AG133" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AH133" s="1" t="s">
+      <c r="AH133" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AI133" s="1" t="s">
+      <c r="AI133" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AJ133" s="1" t="s">
+      <c r="AJ133" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AK133" s="1" t="s">
+      <c r="AK133" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="AL133" s="1" t="s">
+      <c r="AL133" s="12" t="s">
         <v>18</v>
       </c>
       <c r="AM133" s="1"/>
@@ -13778,7 +13818,7 @@
       <c r="CB133" s="3"/>
       <c r="CC133" s="3"/>
       <c r="CD133" s="3"/>
-      <c r="CG133" s="3">
+      <c r="CG133" s="13">
         <v>131</v>
       </c>
       <c r="CH133" s="3"/>
@@ -13868,127 +13908,127 @@
       <c r="CC134" s="3"/>
       <c r="CD134" s="3"/>
       <c r="CG134" s="3"/>
-      <c r="CH134" s="3" t="s">
-        <v>208</v>
+      <c r="CH134" s="13" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="135" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B135" s="2">
         <v>132</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="H135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="I135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="J135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="K135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="L135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="M135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="N135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="O135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="P135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="R135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="S135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="T135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="U135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="V135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="W135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="X135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="Y135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="Z135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AA135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AB135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AC135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AD135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AE135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AF135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AG135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AH135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AI135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AJ135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AK135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AL135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AM135" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AN135" s="1" t="s">
-        <v>235</v>
+      <c r="C135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="D135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="E135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="F135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="G135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="H135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="I135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="J135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="K135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="L135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="M135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="N135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="O135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="P135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="R135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="S135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="T135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="U135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="V135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="W135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="X135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AD135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AF135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AJ135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AK135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AL135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AM135" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN135" s="12" t="s">
+        <v>228</v>
       </c>
       <c r="AO135" s="1"/>
       <c r="AP135" s="1"/>
@@ -14008,85 +14048,85 @@
       <c r="BD135" s="3"/>
       <c r="BE135" s="3"/>
       <c r="BF135" s="3"/>
-      <c r="BG135" s="3">
+      <c r="BG135" s="13">
         <v>134</v>
       </c>
-      <c r="BH135" s="3">
+      <c r="BH135" s="13">
         <v>134</v>
       </c>
-      <c r="BI135" s="3">
+      <c r="BI135" s="13">
         <v>134</v>
       </c>
-      <c r="BJ135" s="3">
+      <c r="BJ135" s="13">
         <v>134</v>
       </c>
-      <c r="BK135" s="3">
+      <c r="BK135" s="13">
         <v>134</v>
       </c>
-      <c r="BL135" s="3">
+      <c r="BL135" s="13">
         <v>134</v>
       </c>
-      <c r="BM135" s="3">
+      <c r="BM135" s="13">
         <v>134</v>
       </c>
-      <c r="BN135" s="3">
+      <c r="BN135" s="13">
         <v>134</v>
       </c>
-      <c r="BO135" s="3">
+      <c r="BO135" s="13">
         <v>134</v>
       </c>
-      <c r="BP135" s="3">
+      <c r="BP135" s="13">
         <v>134</v>
       </c>
-      <c r="BQ135" s="3">
+      <c r="BQ135" s="13">
         <v>134</v>
       </c>
-      <c r="BR135" s="3">
+      <c r="BR135" s="13">
         <v>134</v>
       </c>
-      <c r="BS135" s="3">
+      <c r="BS135" s="13">
         <v>134</v>
       </c>
-      <c r="BT135" s="3">
+      <c r="BT135" s="13">
         <v>134</v>
       </c>
-      <c r="BU135" s="3">
+      <c r="BU135" s="13">
         <v>134</v>
       </c>
-      <c r="BV135" s="3">
+      <c r="BV135" s="13">
         <v>134</v>
       </c>
-      <c r="BW135" s="3">
+      <c r="BW135" s="13">
         <v>134</v>
       </c>
-      <c r="BX135" s="3">
+      <c r="BX135" s="13">
         <v>134</v>
       </c>
-      <c r="BY135" s="3">
+      <c r="BY135" s="13">
         <v>134</v>
       </c>
-      <c r="BZ135" s="3">
+      <c r="BZ135" s="13">
         <v>134</v>
       </c>
-      <c r="CA135" s="3">
+      <c r="CA135" s="13">
         <v>134</v>
       </c>
-      <c r="CB135" s="3">
+      <c r="CB135" s="13">
         <v>134</v>
       </c>
-      <c r="CC135" s="3">
+      <c r="CC135" s="13">
         <v>134</v>
       </c>
-      <c r="CD135" s="3">
+      <c r="CD135" s="13">
         <v>134</v>
       </c>
-      <c r="CE135" s="3">
+      <c r="CE135" s="13">
         <v>134</v>
       </c>
-      <c r="CF135" s="3">
+      <c r="CF135" s="13">
         <v>134</v>
       </c>
-      <c r="CG135" s="3">
+      <c r="CG135" s="13">
         <v>133</v>
       </c>
       <c r="CH135" s="3"/>
@@ -14176,127 +14216,127 @@
       <c r="CC136" s="3"/>
       <c r="CD136" s="3"/>
       <c r="CG136" s="3"/>
-      <c r="CH136" s="3" t="s">
-        <v>112</v>
+      <c r="CH136" s="13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="137" spans="2:86" x14ac:dyDescent="0.25">
       <c r="B137" s="2">
         <v>134</v>
       </c>
-      <c r="C137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="H137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="I137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="J137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="K137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="L137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="M137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="N137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="O137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="P137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="R137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="S137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="T137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="U137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="V137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="W137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="X137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="Y137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="Z137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AA137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AB137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AC137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AD137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AE137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AF137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AG137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AH137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AI137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AJ137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AK137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AL137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AM137" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="AN137" s="1" t="s">
-        <v>235</v>
+      <c r="C137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="D137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="E137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="F137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="G137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="H137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="I137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="J137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="K137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="L137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="M137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="N137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="O137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="P137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="R137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="S137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="T137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="U137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="V137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="W137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="X137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="Y137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AC137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AD137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AF137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AH137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AI137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AJ137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AK137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AL137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AM137" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AN137" s="12" t="s">
+        <v>228</v>
       </c>
       <c r="AO137" s="1"/>
       <c r="AP137" s="1"/>
@@ -14316,85 +14356,85 @@
       <c r="BD137" s="3"/>
       <c r="BE137" s="3"/>
       <c r="BF137" s="3"/>
-      <c r="BG137" s="3">
+      <c r="BG137" s="13">
         <v>134</v>
       </c>
-      <c r="BH137" s="3">
+      <c r="BH137" s="13">
         <v>134</v>
       </c>
-      <c r="BI137" s="3">
+      <c r="BI137" s="13">
         <v>134</v>
       </c>
-      <c r="BJ137" s="3">
+      <c r="BJ137" s="13">
         <v>134</v>
       </c>
-      <c r="BK137" s="3">
+      <c r="BK137" s="13">
         <v>134</v>
       </c>
-      <c r="BL137" s="3">
+      <c r="BL137" s="13">
         <v>134</v>
       </c>
-      <c r="BM137" s="3">
+      <c r="BM137" s="13">
         <v>134</v>
       </c>
-      <c r="BN137" s="3">
+      <c r="BN137" s="13">
         <v>134</v>
       </c>
-      <c r="BO137" s="3">
+      <c r="BO137" s="13">
         <v>134</v>
       </c>
-      <c r="BP137" s="3">
+      <c r="BP137" s="13">
         <v>134</v>
       </c>
-      <c r="BQ137" s="3">
+      <c r="BQ137" s="13">
         <v>134</v>
       </c>
-      <c r="BR137" s="3">
+      <c r="BR137" s="13">
         <v>134</v>
       </c>
-      <c r="BS137" s="3">
+      <c r="BS137" s="13">
         <v>134</v>
       </c>
-      <c r="BT137" s="3">
+      <c r="BT137" s="13">
         <v>134</v>
       </c>
-      <c r="BU137" s="3">
+      <c r="BU137" s="13">
         <v>134</v>
       </c>
-      <c r="BV137" s="3">
+      <c r="BV137" s="13">
         <v>134</v>
       </c>
-      <c r="BW137" s="3">
+      <c r="BW137" s="13">
         <v>134</v>
       </c>
-      <c r="BX137" s="3">
+      <c r="BX137" s="13">
         <v>134</v>
       </c>
-      <c r="BY137" s="3">
+      <c r="BY137" s="13">
         <v>134</v>
       </c>
-      <c r="BZ137" s="3">
+      <c r="BZ137" s="13">
         <v>134</v>
       </c>
-      <c r="CA137" s="3">
+      <c r="CA137" s="13">
         <v>134</v>
       </c>
-      <c r="CB137" s="3">
+      <c r="CB137" s="13">
         <v>134</v>
       </c>
-      <c r="CC137" s="3">
+      <c r="CC137" s="13">
         <v>134</v>
       </c>
-      <c r="CD137" s="3">
+      <c r="CD137" s="13">
         <v>134</v>
       </c>
-      <c r="CE137" s="3">
+      <c r="CE137" s="13">
         <v>134</v>
       </c>
-      <c r="CF137" s="3">
+      <c r="CF137" s="13">
         <v>134</v>
       </c>
-      <c r="CG137" s="3">
+      <c r="CG137" s="13">
         <v>135</v>
       </c>
       <c r="CH137" s="3"/>
@@ -14484,8 +14524,8 @@
       <c r="CC138" s="3"/>
       <c r="CD138" s="3"/>
       <c r="CG138" s="3"/>
-      <c r="CH138" s="3" t="s">
-        <v>60</v>
+      <c r="CH138" s="13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="139" spans="2:86" x14ac:dyDescent="0.25">
@@ -14572,7 +14612,7 @@
       <c r="CB139" s="3"/>
       <c r="CC139" s="3"/>
       <c r="CD139" s="3"/>
-      <c r="CG139" s="3">
+      <c r="CG139" s="13">
         <v>137</v>
       </c>
       <c r="CH139" s="3"/>
@@ -14662,8 +14702,8 @@
       <c r="CC140" s="3"/>
       <c r="CD140" s="3"/>
       <c r="CG140" s="3"/>
-      <c r="CH140" s="3" t="s">
-        <v>114</v>
+      <c r="CH140" s="13" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="141" spans="2:86" x14ac:dyDescent="0.25">
@@ -14750,7 +14790,7 @@
       <c r="CB141" s="3"/>
       <c r="CC141" s="3"/>
       <c r="CD141" s="3"/>
-      <c r="CG141" s="3">
+      <c r="CG141" s="13">
         <v>139</v>
       </c>
       <c r="CH141" s="3"/>
@@ -14840,8 +14880,8 @@
       <c r="CC142" s="3"/>
       <c r="CD142" s="3"/>
       <c r="CG142" s="3"/>
-      <c r="CH142" s="3" t="s">
-        <v>115</v>
+      <c r="CH142" s="13" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="143" spans="2:86" x14ac:dyDescent="0.25">
@@ -14928,7 +14968,7 @@
       <c r="CB143" s="3"/>
       <c r="CC143" s="3"/>
       <c r="CD143" s="3"/>
-      <c r="CG143" s="3">
+      <c r="CG143" s="13">
         <v>142</v>
       </c>
       <c r="CH143" s="3"/>
@@ -15018,8 +15058,8 @@
       <c r="CC144" s="3"/>
       <c r="CD144" s="3"/>
       <c r="CG144" s="3"/>
-      <c r="CH144" s="3" t="s">
-        <v>116</v>
+      <c r="CH144" s="13" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="145" spans="2:86" x14ac:dyDescent="0.25">
@@ -15106,7 +15146,7 @@
       <c r="CB145" s="3"/>
       <c r="CC145" s="3"/>
       <c r="CD145" s="3"/>
-      <c r="CG145" s="3">
+      <c r="CG145" s="13">
         <v>143</v>
       </c>
       <c r="CH145" s="3"/>
@@ -15196,8 +15236,8 @@
       <c r="CC146" s="3"/>
       <c r="CD146" s="3"/>
       <c r="CG146" s="3"/>
-      <c r="CH146" s="3" t="s">
-        <v>117</v>
+      <c r="CH146" s="13" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="147" spans="2:86" x14ac:dyDescent="0.25">
@@ -15284,7 +15324,7 @@
       <c r="CB147" s="3"/>
       <c r="CC147" s="3"/>
       <c r="CD147" s="3"/>
-      <c r="CG147" s="3">
+      <c r="CG147" s="13">
         <v>145</v>
       </c>
       <c r="CH147" s="3"/>
@@ -15374,8 +15414,8 @@
       <c r="CC148" s="3"/>
       <c r="CD148" s="3"/>
       <c r="CG148" s="3"/>
-      <c r="CH148" s="3" t="s">
-        <v>118</v>
+      <c r="CH148" s="13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="149" spans="2:86" x14ac:dyDescent="0.25">
@@ -15462,7 +15502,7 @@
       <c r="CB149" s="3"/>
       <c r="CC149" s="3"/>
       <c r="CD149" s="3"/>
-      <c r="CG149" s="3">
+      <c r="CG149" s="13">
         <v>147</v>
       </c>
       <c r="CH149" s="3"/>
@@ -15552,8 +15592,8 @@
       <c r="CC150" s="3"/>
       <c r="CD150" s="3"/>
       <c r="CG150" s="3"/>
-      <c r="CH150" s="3" t="s">
-        <v>119</v>
+      <c r="CH150" s="13" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="151" spans="2:86" x14ac:dyDescent="0.25">
@@ -15609,7 +15649,7 @@
       <c r="AW151" s="1"/>
       <c r="AX151" s="1"/>
       <c r="AY151" s="1"/>
-      <c r="AZ151" s="3">
+      <c r="AZ151" s="13">
         <v>150</v>
       </c>
       <c r="BA151" s="3"/>
@@ -15642,7 +15682,7 @@
       <c r="CB151" s="3"/>
       <c r="CC151" s="3"/>
       <c r="CD151" s="3"/>
-      <c r="CG151" s="3">
+      <c r="CG151" s="13">
         <v>149</v>
       </c>
       <c r="CH151" s="3"/>
@@ -15732,8 +15772,8 @@
       <c r="CC152" s="3"/>
       <c r="CD152" s="3"/>
       <c r="CG152" s="3"/>
-      <c r="CH152" s="3" t="s">
-        <v>120</v>
+      <c r="CH152" s="13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="153" spans="2:86" x14ac:dyDescent="0.25">
@@ -15820,7 +15860,7 @@
       <c r="CB153" s="3"/>
       <c r="CC153" s="3"/>
       <c r="CD153" s="3"/>
-      <c r="CG153" s="3">
+      <c r="CG153" s="13">
         <v>151</v>
       </c>
       <c r="CH153" s="3"/>
@@ -15910,8 +15950,8 @@
       <c r="CC154" s="3"/>
       <c r="CD154" s="3"/>
       <c r="CG154" s="3"/>
-      <c r="CH154" s="3" t="s">
-        <v>121</v>
+      <c r="CH154" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="155" spans="2:86" x14ac:dyDescent="0.25">
@@ -15971,7 +16011,7 @@
       <c r="BA155" s="3"/>
       <c r="BB155" s="3"/>
       <c r="BC155" s="3"/>
-      <c r="BD155" s="3">
+      <c r="BD155" s="13">
         <v>154</v>
       </c>
       <c r="BE155" s="3"/>
@@ -16000,7 +16040,7 @@
       <c r="CB155" s="3"/>
       <c r="CC155" s="3"/>
       <c r="CD155" s="3"/>
-      <c r="CG155" s="3">
+      <c r="CG155" s="13">
         <v>153</v>
       </c>
       <c r="CH155" s="3"/>
@@ -16090,8 +16130,8 @@
       <c r="CC156" s="3"/>
       <c r="CD156" s="3"/>
       <c r="CG156" s="3"/>
-      <c r="CH156" s="3" t="s">
-        <v>122</v>
+      <c r="CH156" s="13" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="157" spans="2:86" x14ac:dyDescent="0.25">
@@ -16178,7 +16218,7 @@
       <c r="CB157" s="3"/>
       <c r="CC157" s="3"/>
       <c r="CD157" s="3"/>
-      <c r="CG157" s="3">
+      <c r="CG157" s="13">
         <v>155</v>
       </c>
       <c r="CH157" s="3"/>
@@ -16268,8 +16308,8 @@
       <c r="CC158" s="3"/>
       <c r="CD158" s="3"/>
       <c r="CG158" s="3"/>
-      <c r="CH158" s="3" t="s">
-        <v>123</v>
+      <c r="CH158" s="13" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="159" spans="2:86" x14ac:dyDescent="0.25">
@@ -16356,7 +16396,7 @@
       <c r="CB159" s="3"/>
       <c r="CC159" s="3"/>
       <c r="CD159" s="3"/>
-      <c r="CG159" s="3">
+      <c r="CG159" s="13">
         <v>157</v>
       </c>
       <c r="CH159" s="3"/>
@@ -16446,8 +16486,8 @@
       <c r="CC160" s="3"/>
       <c r="CD160" s="3"/>
       <c r="CG160" s="3"/>
-      <c r="CH160" s="3" t="s">
-        <v>124</v>
+      <c r="CH160" s="13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="161" spans="2:86" x14ac:dyDescent="0.25">
@@ -16534,7 +16574,7 @@
       <c r="CB161" s="3"/>
       <c r="CC161" s="3"/>
       <c r="CD161" s="3"/>
-      <c r="CG161" s="3">
+      <c r="CG161" s="13">
         <v>159</v>
       </c>
       <c r="CH161" s="3"/>
@@ -16624,8 +16664,8 @@
       <c r="CC162" s="3"/>
       <c r="CD162" s="3"/>
       <c r="CG162" s="3"/>
-      <c r="CH162" s="3" t="s">
-        <v>125</v>
+      <c r="CH162" s="13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="163" spans="2:86" x14ac:dyDescent="0.25">
@@ -16712,7 +16752,7 @@
       <c r="CB163" s="3"/>
       <c r="CC163" s="3"/>
       <c r="CD163" s="3"/>
-      <c r="CG163" s="3">
+      <c r="CG163" s="13">
         <v>161</v>
       </c>
       <c r="CH163" s="3"/>
@@ -16802,8 +16842,8 @@
       <c r="CC164" s="3"/>
       <c r="CD164" s="3"/>
       <c r="CG164" s="3"/>
-      <c r="CH164" s="3" t="s">
-        <v>126</v>
+      <c r="CH164" s="13" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="165" spans="2:86" x14ac:dyDescent="0.25">
@@ -16890,7 +16930,7 @@
       <c r="CB165" s="3"/>
       <c r="CC165" s="3"/>
       <c r="CD165" s="3"/>
-      <c r="CG165" s="3">
+      <c r="CG165" s="13">
         <v>163</v>
       </c>
       <c r="CH165" s="3"/>
@@ -16980,8 +17020,8 @@
       <c r="CC166" s="3"/>
       <c r="CD166" s="3"/>
       <c r="CG166" s="3"/>
-      <c r="CH166" s="3" t="s">
-        <v>127</v>
+      <c r="CH166" s="13" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="167" spans="2:86" x14ac:dyDescent="0.25">
@@ -17068,7 +17108,7 @@
       <c r="CB167" s="3"/>
       <c r="CC167" s="3"/>
       <c r="CD167" s="3"/>
-      <c r="CG167" s="3">
+      <c r="CG167" s="13">
         <v>165</v>
       </c>
       <c r="CH167" s="3"/>
@@ -17158,8 +17198,8 @@
       <c r="CC168" s="3"/>
       <c r="CD168" s="3"/>
       <c r="CG168" s="3"/>
-      <c r="CH168" s="3" t="s">
-        <v>128</v>
+      <c r="CH168" s="13" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="169" spans="2:86" x14ac:dyDescent="0.25">
@@ -17246,7 +17286,7 @@
       <c r="CB169" s="3"/>
       <c r="CC169" s="3"/>
       <c r="CD169" s="3"/>
-      <c r="CG169" s="3">
+      <c r="CG169" s="13">
         <v>167</v>
       </c>
       <c r="CH169" s="3"/>
@@ -17336,8 +17376,8 @@
       <c r="CC170" s="3"/>
       <c r="CD170" s="3"/>
       <c r="CG170" s="3"/>
-      <c r="CH170" s="3" t="s">
-        <v>129</v>
+      <c r="CH170" s="13" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="171" spans="2:86" x14ac:dyDescent="0.25">
@@ -17424,7 +17464,7 @@
       <c r="CB171" s="3"/>
       <c r="CC171" s="3"/>
       <c r="CD171" s="3"/>
-      <c r="CG171" s="3">
+      <c r="CG171" s="13">
         <v>169</v>
       </c>
       <c r="CH171" s="3"/>
@@ -17514,8 +17554,8 @@
       <c r="CC172" s="3"/>
       <c r="CD172" s="3"/>
       <c r="CG172" s="3"/>
-      <c r="CH172" s="3" t="s">
-        <v>130</v>
+      <c r="CH172" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="173" spans="2:86" x14ac:dyDescent="0.25">
@@ -17602,7 +17642,7 @@
       <c r="CB173" s="3"/>
       <c r="CC173" s="3"/>
       <c r="CD173" s="3"/>
-      <c r="CG173" s="3">
+      <c r="CG173" s="13">
         <v>171</v>
       </c>
       <c r="CH173" s="3"/>
@@ -17636,8 +17676,8 @@
       <c r="CC174" s="3"/>
       <c r="CD174" s="3"/>
       <c r="CG174" s="3"/>
-      <c r="CH174" s="3" t="s">
-        <v>131</v>
+      <c r="CH174" s="13" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="175" spans="2:86" x14ac:dyDescent="0.25">
@@ -18383,8 +18423,15 @@
       <c r="BX208" s="3"/>
     </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{817BAEF7-F0B5-4F57-B3D7-04F4E674B0EF}" scale="85" topLeftCell="BQ1">
+      <selection activeCell="B2" sqref="B2:CH2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" copies="7" r:id="rId1"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" copies="7" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" copies="7" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>